<commit_message>
power and assault updates
Power and price corrected
can't open chest & co during assault in any base
champions can't open enchant table and anvil
champion can't interact with his equipment
regen desactivated
stuff unbreackable
champion glowing under y = 64
</commit_message>
<xml_diff>
--- a/powerandprice.xlsx
+++ b/powerandprice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projets Prog\GitHub\FlamboyantSurvivalRumble\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flamboyant\Documents\GitHub\FlamboyantSurvivalRumble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D25FDF5-1926-4E29-A373-DF876417F3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A280EC-A1E7-4EEF-8258-001649D3AD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE0511E6-2CB4-423D-9419-747EC9372C3E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CE0511E6-2CB4-423D-9419-747EC9372C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="112">
   <si>
     <t>EQUIPMENT</t>
   </si>
@@ -317,6 +317,84 @@
   </si>
   <si>
     <t>Les assaillants perdent|leur bouclier</t>
+  </si>
+  <si>
+    <t>Effet Force 1</t>
+  </si>
+  <si>
+    <t>Effet Force 1|-&gt; Effet Force 2</t>
+  </si>
+  <si>
+    <t>Effet Force 2</t>
+  </si>
+  <si>
+    <t>Effet Résistance 1</t>
+  </si>
+  <si>
+    <t>Effet Résistance 1|-&gt;Effet Résistance 2</t>
+  </si>
+  <si>
+    <t>Effet Résistance 2</t>
+  </si>
+  <si>
+    <t>Effet Speed 1</t>
+  </si>
+  <si>
+    <t>Effet Speed 1|-&gt;Effet Speed 2</t>
+  </si>
+  <si>
+    <t>Effet Speed 2</t>
+  </si>
+  <si>
+    <t>Effet Jump 1</t>
+  </si>
+  <si>
+    <t>Effet Jump 1|-&gt;Effet Jump 2</t>
+  </si>
+  <si>
+    <t>Effet Jump 2</t>
+  </si>
+  <si>
+    <t>Effet Résistance au Feu</t>
+  </si>
+  <si>
+    <t>Les mobs n'attaquent pas|le capitaine</t>
+  </si>
+  <si>
+    <t>Les assaillants à moins|de 30 blocs sont en|surbrillance</t>
+  </si>
+  <si>
+    <t>Pas de dégât de chute</t>
+  </si>
+  <si>
+    <t>Envoi les ennemis proches|dans les airs</t>
+  </si>
+  <si>
+    <t>Invoque des mobs près|des assaillants</t>
+  </si>
+  <si>
+    <t>Fait un grand saut</t>
+  </si>
+  <si>
+    <t>Le prochain bloc posé|par un assaillant explose</t>
+  </si>
+  <si>
+    <t>Enferme un assaillant dasn|une prison d'obsidienne</t>
+  </si>
+  <si>
+    <t>Fait disparaitre tous les|blocs sous les pieds du|capitaine jusqu'à la couche 0</t>
+  </si>
+  <si>
+    <t>Intervertit la position|des assaillants</t>
+  </si>
+  <si>
+    <t>A 0 cœurs récupère|3 cœurs + 2 d'abso|un assaillant allié perd|tout son équipement</t>
+  </si>
+  <si>
+    <t>A 5 cœurs les assaillants|subissent un poison jusqu'à|5 cœurs max</t>
+  </si>
+  <si>
+    <t>A 2 cœurs teleporte|le capitaine au point le|plus haut de sa position</t>
   </si>
 </sst>
 </file>
@@ -369,19 +447,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -428,6 +502,9 @@
         </left>
       </border>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -448,7 +525,7 @@
     <tableColumn id="1" xr3:uid="{6C46DAC8-560F-4C0E-A953-82498D3166C8}" name="Effect enum"/>
     <tableColumn id="4" xr3:uid="{B62B264B-1F8F-4BBC-8B19-926F7AB01D18}" name="Name"/>
     <tableColumn id="3" xr3:uid="{2BB105C0-6BF3-4E12-8B7F-B478C2163ABD}" name="Material"/>
-    <tableColumn id="2" xr3:uid="{81E8D61A-20DE-4A20-B69C-D00038FA727E}" name="Colonne2" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{81E8D61A-20DE-4A20-B69C-D00038FA727E}" name="Colonne2" dataDxfId="3">
       <calculatedColumnFormula array="1">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A2,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -457,14 +534,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2796FCD-5C41-4103-9DBE-EF9DFB53ACDC}" name="Tableau3" displayName="Tableau3" ref="A1:E39" totalsRowShown="0" tableBorderDxfId="3">
-  <autoFilter ref="A1:E39" xr:uid="{D2796FCD-5C41-4103-9DBE-EF9DFB53ACDC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2796FCD-5C41-4103-9DBE-EF9DFB53ACDC}" name="Tableau3" displayName="Tableau3" ref="A1:E47" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="A1:E47" xr:uid="{D2796FCD-5C41-4103-9DBE-EF9DFB53ACDC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8F341F71-2B53-409D-83BA-B4D0D14E06C7}" name="Effect enum" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{8F341F71-2B53-409D-83BA-B4D0D14E06C7}" name="Effect enum" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{34497726-02A4-4E64-A7CC-3DEB45AF79C3}" name="Level"/>
     <tableColumn id="4" xr3:uid="{9E224BC4-229E-4504-8989-4328D16E45D0}" name="Price"/>
     <tableColumn id="3" xr3:uid="{140BA913-0257-4365-B79F-C2928DB5893B}" name="Description"/>
-    <tableColumn id="5" xr3:uid="{E43C4AE8-AD62-4C66-B86F-B4E6ED3E509A}" name="Quoted" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{E43C4AE8-AD62-4C66-B86F-B4E6ED3E509A}" name="Quoted" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -791,18 +868,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF46C1E-7778-41FA-B71C-06D6E1FA3772}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D2:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -816,7 +893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -831,7 +908,7 @@
         <v>new ChampionPower(ChampionPowerType.EQUIPMENT, Arrays.asList(new LevelDescription(10, Arrays.asList("Equipement Cuir et Pierre")), new LevelDescription(20, Arrays.asList("Equipement Cuir et Pierre", "-&gt; Equipement Or")), new LevelDescription(50, Arrays.asList("Equipement Or", "-&gt; Equipement Fer")), new LevelDescription(100, Arrays.asList("Equipement Fer", "-&gt; Equipement Diamant")), new LevelDescription(200, Arrays.asList("Equipement Diamant", "-&gt; Equipement Netherite")), new LevelDescription(200, Arrays.asList("Equipement Netherite", "-&gt; Protection 1")), new LevelDescription(300, Arrays.asList("Protection 1", "-&gt; Protection 2")), new LevelDescription(400, Arrays.asList("Protection 2", "-&gt; Protection 3")), new LevelDescription(500, Arrays.asList("Protection 3", "-&gt;Protection 4")), new LevelDescription(200, Arrays.asList("Protection 4", "-&gt; Full Enchant")), new LevelDescription(0, Arrays.asList("Full Enchant"))), "Equipement", Material.LEATHER_CHESTPLATE),</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -846,7 +923,7 @@
         <v>new ChampionPower(ChampionPowerType.BOW, Arrays.asList(new LevelDescription(50, Arrays.asList("Arc + 2 stacks de Fleches")), new LevelDescription(100, Arrays.asList("Arc + 2 stacks de Fleches", "-&gt;Power 1")), new LevelDescription(300, Arrays.asList("Power 1", "-&gt; Power 3 + 1 stack de Flèches")), new LevelDescription(200, Arrays.asList("Power 3 + 1 stack de Flèches", "-&gt; Power 4")), new LevelDescription(500, Arrays.asList("Power 4", "-&gt; Full Enchant")), new LevelDescription(0, Arrays.asList("Full Enchant"))), "Archerie", Material.BOW),</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -861,7 +938,7 @@
         <v>new ChampionPower(ChampionPowerType.ENDERCHEST_STUFF, Arrays.asList(new LevelDescription(500, Arrays.asList("Recoit les items de", "son Ender Chest"))), "Enderchest Drop", Material.ENDER_CHEST),</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -876,7 +953,7 @@
         <v>new ChampionPower(ChampionPowerType.NO_SHIELD, Arrays.asList(new LevelDescription(2000, Arrays.asList("Les assaillants perdent", "leur bouclier"))), "No Shield", Material.SHIELD),</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -888,10 +965,10 @@
       </c>
       <c r="D6" t="str" cm="1">
         <f t="array" ref="D6">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A6,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.EFFECT_STRENGH, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Effet Force", Material.POTION),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.EFFECT_STRENGH, Arrays.asList(new LevelDescription(500, Arrays.asList("Effet Force 1")), new LevelDescription(2000, Arrays.asList("Effet Force 1", "-&gt; Effet Force 2")), new LevelDescription(0, Arrays.asList("Effet Force 2"))), "Effet Force", Material.POTION),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -903,10 +980,10 @@
       </c>
       <c r="D7" t="str" cm="1">
         <f t="array" ref="D7">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A7,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.EFFECT_RESISTANCE, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Effet Resistance", Material.POTION),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.EFFECT_RESISTANCE, Arrays.asList(new LevelDescription(500, Arrays.asList("Effet Résistance 1")), new LevelDescription(2000, Arrays.asList("Effet Résistance 1", "-&gt;Effet Résistance 2")), new LevelDescription(0, Arrays.asList("Effet Résistance 2"))), "Effet Resistance", Material.POTION),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -918,10 +995,10 @@
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" ref="D8">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A8,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.EFFECT_SPEED, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Effet Vitesse", Material.POTION),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.EFFECT_SPEED, Arrays.asList(new LevelDescription(500, Arrays.asList("Effet Speed 1")), new LevelDescription(1000, Arrays.asList("Effet Speed 1", "-&gt;Effet Speed 2")), new LevelDescription(0, Arrays.asList("Effet Speed 2"))), "Effet Vitesse", Material.POTION),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -933,10 +1010,10 @@
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" ref="D9">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A9,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.EFFECT_JUMP, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Effet Saut", Material.POTION),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.EFFECT_JUMP, Arrays.asList(new LevelDescription(500, Arrays.asList("Effet Jump 1")), new LevelDescription(1000, Arrays.asList("Effet Jump 1", "-&gt;Effet Jump 2")), new LevelDescription(0, Arrays.asList("Effet Jump 2"))), "Effet Saut", Material.POTION),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -948,10 +1025,10 @@
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" ref="D10">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A10,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.EFFECT_FIRE_RESISTANCE, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Effet Resistance au Feu", Material.BLAZE_POWDER),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.EFFECT_FIRE_RESISTANCE, Arrays.asList(new LevelDescription(2000, Arrays.asList("Effet Résistance au Feu"))), "Effet Resistance au Feu", Material.BLAZE_POWDER),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -963,10 +1040,10 @@
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" ref="D11">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A11,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.EFFECT_WATER_BREATHING, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Effet Respiration", Material.CONDUIT),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.EFFECT_WATER_BREATHING, Arrays.asList(new LevelDescription(500, Arrays.asList("Effet Respiration"))), "Effet Respiration", Material.CONDUIT),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -978,10 +1055,10 @@
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" ref="D12">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A12,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.MOB_FRIEND, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Ami des Mobs", Material.CREEPER_HEAD),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.MOB_FRIEND, Arrays.asList(new LevelDescription(500, Arrays.asList("Les mobs n'attaquent pas", "le capitaine"))), "Ami des Mobs", Material.CREEPER_HEAD),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -993,10 +1070,10 @@
       </c>
       <c r="D13" t="str" cm="1">
         <f t="array" ref="D13">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A13,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.ENNEMY_DETECTION, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Detection des assaillants", Material.TARGET),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.ENNEMY_DETECTION, Arrays.asList(new LevelDescription(2000, Arrays.asList("Les assaillants à moins", "de 30 blocs sont en", "surbrillance"))), "Detection des assaillants", Material.TARGET),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1008,10 +1085,10 @@
       </c>
       <c r="D14" t="str" cm="1">
         <f t="array" ref="D14">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A14,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.NO_FALL_DAMAGE, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Pas de chute", Material.FEATHER),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.NO_FALL_DAMAGE, Arrays.asList(new LevelDescription(2000, Arrays.asList("Pas de dégât de chute"))), "Pas de chute", Material.FEATHER),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1023,10 +1100,10 @@
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" ref="D15">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A15,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.SPELL_SCREAM, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Sort : Cri d'Effroi", Material.WRITABLE_BOOK),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.SPELL_SCREAM, Arrays.asList(new LevelDescription(1000, Arrays.asList("Envoi les ennemis proches", "dans les airs"))), "Sort : Cri d'Effroi", Material.WRITABLE_BOOK),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1038,10 +1115,10 @@
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" ref="D16">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A16,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.SPELL_SUMMON, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Sort : Invocation", Material.WRITABLE_BOOK),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.SPELL_SUMMON, Arrays.asList(new LevelDescription(1000, Arrays.asList("Invoque des mobs près", "des assaillants"))), "Sort : Invocation", Material.WRITABLE_BOOK),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1053,10 +1130,10 @@
       </c>
       <c r="D17" t="str" cm="1">
         <f t="array" ref="D17">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A17,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.SPELL_JUMP, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Sort : Saut", Material.WRITABLE_BOOK),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.SPELL_JUMP, Arrays.asList(new LevelDescription(1000, Arrays.asList("Fait un grand saut"))), "Sort : Saut", Material.WRITABLE_BOOK),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1068,10 +1145,10 @@
       </c>
       <c r="D18" t="str" cm="1">
         <f t="array" ref="D18">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A18,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.SPELL_EXPLOSIVE_PUN, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Sort : Farce Explosive", Material.WRITABLE_BOOK),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.SPELL_EXPLOSIVE_PUN, Arrays.asList(new LevelDescription(2000, Arrays.asList("Le prochain bloc posé", "par un assaillant explose"))), "Sort : Farce Explosive", Material.WRITABLE_BOOK),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1083,10 +1160,10 @@
       </c>
       <c r="D19" t="str" cm="1">
         <f t="array" ref="D19">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A19,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.SPELL_JAIL, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Sort : Prison", Material.WRITABLE_BOOK),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.SPELL_JAIL, Arrays.asList(new LevelDescription(2000, Arrays.asList("Enferme un assaillant dasn", "une prison d'obsidienne"))), "Sort : Prison", Material.WRITABLE_BOOK),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1098,10 +1175,10 @@
       </c>
       <c r="D20" t="str" cm="1">
         <f t="array" ref="D20">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A20,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.SPELL_ADIOS, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Sort : Adios!", Material.WRITABLE_BOOK),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.SPELL_ADIOS, Arrays.asList(new LevelDescription(2000, Arrays.asList("Fait disparaitre tous les", "blocs sous les pieds du", "capitaine jusqu'à la couche 0"))), "Sort : Adios!", Material.WRITABLE_BOOK),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1113,10 +1190,10 @@
       </c>
       <c r="D21" t="str" cm="1">
         <f t="array" ref="D21">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A21,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.SPELL_SHUFFLE, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Sort : Shuffle", Material.WRITABLE_BOOK),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.SPELL_SHUFFLE, Arrays.asList(new LevelDescription(1000, Arrays.asList("Intervertit la position", "des assaillants"))), "Sort : Shuffle", Material.WRITABLE_BOOK),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1128,10 +1205,10 @@
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" ref="D22">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A22,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.COME_BACK_REVIVE, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Sauvetage", Material.TOTEM_OF_UNDYING),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.COME_BACK_REVIVE, Arrays.asList(new LevelDescription(2000, Arrays.asList("A 0 cœurs récupère", "3 cœurs + 2 d'abso", "un assaillant allié perd", "tout son équipement"))), "Sauvetage", Material.TOTEM_OF_UNDYING),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1143,10 +1220,10 @@
       </c>
       <c r="D23" t="str" cm="1">
         <f t="array" ref="D23">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A23,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.COME_BACK_BALANCE, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Equilibre", Material.DAMAGED_ANVIL),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>new ChampionPower(ChampionPowerType.COME_BACK_BALANCE, Arrays.asList(new LevelDescription(4000, Arrays.asList("A 5 cœurs les assaillants", "subissent un poison jusqu'à", "5 cœurs max"))), "Equilibre", Material.DAMAGED_ANVIL),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1158,7 +1235,7 @@
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" ref="D24">_xlfn.CONCAT("new ChampionPower(ChampionPowerType.",A24,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPower(ChampionPowerType.COME_BACK_JUMP_SCARE, Arrays.asList(new LevelDescription(, Arrays.asList(""))), "Trouille", Material.JACK_O_LANTERN),</v>
+        <v>new ChampionPower(ChampionPowerType.COME_BACK_JUMP_SCARE, Arrays.asList(new LevelDescription(2000, Arrays.asList("A 2 cœurs teleporte", "le capitaine au point le", "plus haut de sa position"))), "Trouille", Material.JACK_O_LANTERN),</v>
       </c>
     </row>
   </sheetData>
@@ -1172,21 +1249,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D50422-CDA8-489F-BE44-C27697BFE280}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -1203,7 +1280,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1298,7 @@
         <v>new LevelDescription(10, Arrays.asList("Equipement Cuir et Pierre"))</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1317,7 @@
         <v>new LevelDescription(20, Arrays.asList("Equipement Cuir et Pierre", "-&gt; Equipement Or"))</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1254,12 +1331,12 @@
       <c r="D4" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="3" t="str">
+      <c r="E4" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(50, Arrays.asList("Equipement Or", "-&gt; Equipement Fer"))</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1273,12 +1350,12 @@
       <c r="D5" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="3" t="str">
+      <c r="E5" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(100, Arrays.asList("Equipement Fer", "-&gt; Equipement Diamant"))</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1292,12 +1369,12 @@
       <c r="D6" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="3" t="str">
+      <c r="E6" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(200, Arrays.asList("Equipement Diamant", "-&gt; Equipement Netherite"))</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1311,12 +1388,12 @@
       <c r="D7" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="3" t="str">
+      <c r="E7" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(200, Arrays.asList("Equipement Netherite", "-&gt; Protection 1"))</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,12 +1407,12 @@
       <c r="D8" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="3" t="str">
+      <c r="E8" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(300, Arrays.asList("Protection 1", "-&gt; Protection 2"))</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1349,12 +1426,12 @@
       <c r="D9" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="3" t="str">
+      <c r="E9" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(400, Arrays.asList("Protection 2", "-&gt; Protection 3"))</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1368,12 +1445,12 @@
       <c r="D10" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="3" t="str">
+      <c r="E10" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(500, Arrays.asList("Protection 3", "-&gt;Protection 4"))</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1387,12 +1464,12 @@
       <c r="D11" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="3" t="str">
+      <c r="E11" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(200, Arrays.asList("Protection 4", "-&gt; Full Enchant"))</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1405,12 +1482,12 @@
       <c r="D12" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="3" t="str">
+      <c r="E12" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(0, Arrays.asList("Full Enchant"))</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -1428,7 +1505,7 @@
         <v>new LevelDescription(50, Arrays.asList("Arc + 2 stacks de Fleches"))</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1442,12 +1519,12 @@
       <c r="D14" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="3" t="str">
+      <c r="E14" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(100, Arrays.asList("Arc + 2 stacks de Fleches", "-&gt;Power 1"))</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -1461,12 +1538,12 @@
       <c r="D15" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="3" t="str">
+      <c r="E15" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(300, Arrays.asList("Power 1", "-&gt; Power 3 + 1 stack de Flèches"))</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -1480,12 +1557,12 @@
       <c r="D16" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="3" t="str">
+      <c r="E16" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(200, Arrays.asList("Power 3 + 1 stack de Flèches", "-&gt; Power 4"))</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -1499,12 +1576,12 @@
       <c r="D17" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="3" t="str">
+      <c r="E17" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(500, Arrays.asList("Power 4", "-&gt; Full Enchant"))</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
@@ -1517,12 +1594,12 @@
       <c r="D18" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="3" t="str">
+      <c r="E18" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
         <v>new LevelDescription(0, Arrays.asList("Full Enchant"))</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1540,7 +1617,7 @@
         <v>new LevelDescription(500, Arrays.asList("Recoit les items de", "son Ender Chest"))</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1558,232 +1635,490 @@
         <v>new LevelDescription(2000, Arrays.asList("Les assaillants perdent", "leur bouclier"))</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
+      <c r="C21">
+        <v>500</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
       <c r="E21" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+        <v>new LevelDescription(500, Arrays.asList("Effet Force 1"))</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>2000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(2000, Arrays.asList("Effet Force 1", "-&gt; Effet Force 2"))</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(0, Arrays.asList("Effet Force 2"))</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>500</v>
+      </c>
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(500, Arrays.asList("Effet Résistance 1"))</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>2000</v>
+      </c>
+      <c r="D25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(2000, Arrays.asList("Effet Résistance 1", "-&gt;Effet Résistance 2"))</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(0, Arrays.asList("Effet Résistance 2"))</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>500</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(500, Arrays.asList("Effet Speed 1"))</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>1000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(1000, Arrays.asList("Effet Speed 1", "-&gt;Effet Speed 2"))</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(0, Arrays.asList("Effet Speed 2"))</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>500</v>
+      </c>
+      <c r="D30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(500, Arrays.asList("Effet Jump 1"))</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>1000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(1000, Arrays.asList("Effet Jump 1", "-&gt;Effet Jump 2"))</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(0, Arrays.asList("Effet Jump 2"))</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>2000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(2000, Arrays.asList("Effet Résistance au Feu"))</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>500</v>
+      </c>
+      <c r="D34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(500, Arrays.asList("Effet Respiration"))</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>500</v>
+      </c>
+      <c r="D35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(500, Arrays.asList("Les mobs n'attaquent pas", "le capitaine"))</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>2000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(2000, Arrays.asList("Les assaillants à moins", "de 30 blocs sont en", "surbrillance"))</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>2000</v>
+      </c>
+      <c r="D37" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(2000, Arrays.asList("Pas de dégât de chute"))</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="E30" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1000</v>
+      </c>
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(1000, Arrays.asList("Envoi les ennemis proches", "dans les airs"))</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1000</v>
+      </c>
+      <c r="D39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(1000, Arrays.asList("Invoque des mobs près", "des assaillants"))</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1000</v>
+      </c>
+      <c r="D40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(1000, Arrays.asList("Fait un grand saut"))</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="E33" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>2000</v>
+      </c>
+      <c r="D41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(2000, Arrays.asList("Le prochain bloc posé", "par un assaillant explose"))</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="E34" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>2000</v>
+      </c>
+      <c r="D42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E42" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(2000, Arrays.asList("Enferme un assaillant dasn", "une prison d'obsidienne"))</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="E35" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>2000</v>
+      </c>
+      <c r="D43" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(2000, Arrays.asList("Fait disparaitre tous les", "blocs sous les pieds du", "capitaine jusqu'à la couche 0"))</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="E36" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1000</v>
+      </c>
+      <c r="D44" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(1000, Arrays.asList("Intervertit la position", "des assaillants"))</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>2000</v>
+      </c>
+      <c r="D45" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(2000, Arrays.asList("A 0 cœurs récupère", "3 cœurs + 2 d'abso", "un assaillant allié perd", "tout son équipement"))</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>4000</v>
+      </c>
+      <c r="D46" t="s">
+        <v>110</v>
+      </c>
+      <c r="E46" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(4000, Arrays.asList("A 5 cœurs les assaillants", "subissent un poison jusqu'à", "5 cœurs max"))</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="E39" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(, Arrays.asList(""))</v>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>2000</v>
+      </c>
+      <c r="D47" t="s">
+        <v>111</v>
+      </c>
+      <c r="E47" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
+        <v>new LevelDescription(2000, Arrays.asList("A 2 cœurs teleporte", "le capitaine au point le", "plus haut de sa position"))</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debug death management + shop
</commit_message>
<xml_diff>
--- a/powerandprice.xlsx
+++ b/powerandprice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projets Prog\GitHub\FlamboyantSurvivalRumble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF248C7B-330A-4373-9A98-3A95F7D243B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D12A3B-3DD8-4B43-806E-378716FDFA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE0511E6-2CB4-423D-9419-747EC9372C3E}"/>
   </bookViews>
@@ -37,9 +37,10 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -50,16 +51,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="113">
   <si>
     <t>EQUIPMENT</t>
   </si>
@@ -395,6 +410,9 @@
   </si>
   <si>
     <t>Enferme tous les  assaillants|dans une prison d'obsidienne</t>
+  </si>
+  <si>
+    <t>ENNEMIES_DETECTION</t>
   </si>
 </sst>
 </file>
@@ -518,6 +536,64 @@
 </styleSheet>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>13</v>
+    <v>3</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB36BB41-6156-43AD-97FF-A9DAF9EB0FFB}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0">
   <autoFilter ref="A1:D24" xr:uid="{DB36BB41-6156-43AD-97FF-A9DAF9EB0FFB}"/>
@@ -542,7 +618,7 @@
     <tableColumn id="4" xr3:uid="{9E224BC4-229E-4504-8989-4328D16E45D0}" name="Price"/>
     <tableColumn id="3" xr3:uid="{140BA913-0257-4365-B79F-C2928DB5893B}" name="Description"/>
     <tableColumn id="5" xr3:uid="{E43C4AE8-AD62-4C66-B86F-B4E6ED3E509A}" name="Quoted" dataDxfId="0">
-      <calculatedColumnFormula>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -869,7 +945,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +981,7 @@
       </c>
       <c r="D2" t="str" cm="1">
         <f t="array" ref="D2">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A2,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.EQUIPMENT, Arrays.asList(new LevelDescription(10, Arrays.asList("Equipement Cuir et Pierre")), new LevelDescription(20, Arrays.asList("Equipement Cuir et Pierre", "-&gt; Equipement Or")), new LevelDescription(50, Arrays.asList("Equipement Or", "-&gt; Equipement Fer")), new LevelDescription(100, Arrays.asList("Equipement Fer", "-&gt; Equipement Diamant")), new LevelDescription(200, Arrays.asList("Equipement Diamant", "-&gt; Equipement Netherite")), new LevelDescription(200, Arrays.asList("Equipement Netherite", "-&gt; Protection 1")), new LevelDescription(300, Arrays.asList("Protection 1", "-&gt; Protection 2")), new LevelDescription(400, Arrays.asList("Protection 2", "-&gt; Protection 3")), new LevelDescription(500, Arrays.asList("Protection 3", "-&gt;Protection 4")), new LevelDescription(200, Arrays.asList("Protection 4", "-&gt; Full Enchant")), new LevelDescription(0, Arrays.asList("Full Enchant"))), "Equipement", Material.LEATHER_CHESTPLATE),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.EQUIPMENT, Arrays.asList(new LevelDescription(10, new ArrayList&lt;&gt;(Arrays.asList("Equipement Cuir et Pierre"))), new LevelDescription(20, new ArrayList&lt;&gt;(Arrays.asList("Equipement Cuir et Pierre", "-&gt; Equipement Or"))), new LevelDescription(50, new ArrayList&lt;&gt;(Arrays.asList("Equipement Or", "-&gt; Equipement Fer"))), new LevelDescription(100, new ArrayList&lt;&gt;(Arrays.asList("Equipement Fer", "-&gt; Equipement Diamant"))), new LevelDescription(200, new ArrayList&lt;&gt;(Arrays.asList("Equipement Diamant", "-&gt; Equipement Netherite"))), new LevelDescription(200, new ArrayList&lt;&gt;(Arrays.asList("Equipement Netherite", "-&gt; Protection 1"))), new LevelDescription(300, new ArrayList&lt;&gt;(Arrays.asList("Protection 1", "-&gt; Protection 2"))), new LevelDescription(400, new ArrayList&lt;&gt;(Arrays.asList("Protection 2", "-&gt; Protection 3"))), new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Protection 3", "-&gt;Protection 4"))), new LevelDescription(200, new ArrayList&lt;&gt;(Arrays.asList("Protection 4", "-&gt; Full Enchant"))), new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Full Enchant")))), "Equipement", Material.LEATHER_CHESTPLATE),</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -920,7 +996,7 @@
       </c>
       <c r="D3" t="str" cm="1">
         <f t="array" ref="D3">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A3,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.BOW, Arrays.asList(new LevelDescription(50, Arrays.asList("Arc + 2 stacks de Fleches")), new LevelDescription(100, Arrays.asList("Arc + 2 stacks de Fleches", "-&gt;Power 1")), new LevelDescription(300, Arrays.asList("Power 1", "-&gt; Power 3 + 1 stack de Flèches")), new LevelDescription(200, Arrays.asList("Power 3 + 1 stack de Flèches", "-&gt; Power 4")), new LevelDescription(500, Arrays.asList("Power 4", "-&gt; Full Enchant")), new LevelDescription(0, Arrays.asList("Full Enchant"))), "Archerie", Material.BOW),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.BOW, Arrays.asList(new LevelDescription(50, new ArrayList&lt;&gt;(Arrays.asList("Arc + 2 stacks de Fleches"))), new LevelDescription(100, new ArrayList&lt;&gt;(Arrays.asList("Arc + 2 stacks de Fleches", "-&gt;Power 1"))), new LevelDescription(300, new ArrayList&lt;&gt;(Arrays.asList("Power 1", "-&gt; Power 3 + 1 stack de Flèches"))), new LevelDescription(200, new ArrayList&lt;&gt;(Arrays.asList("Power 3 + 1 stack de Flèches", "-&gt; Power 4"))), new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Power 4", "-&gt; Full Enchant"))), new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Full Enchant")))), "Archerie", Material.BOW),</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -935,7 +1011,7 @@
       </c>
       <c r="D4" t="str" cm="1">
         <f t="array" ref="D4">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A4,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.ENDERCHEST_STUFF, Arrays.asList(new LevelDescription(500, Arrays.asList("Recoit les items de", "son Ender Chest"))), "Enderchest Drop", Material.ENDER_CHEST),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.ENDERCHEST_STUFF, Arrays.asList(new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Recoit les items de", "son Ender Chest")))), "Enderchest Drop", Material.ENDER_CHEST),</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -950,7 +1026,7 @@
       </c>
       <c r="D5" t="str" cm="1">
         <f t="array" ref="D5">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A5,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.NO_SHIELD, Arrays.asList(new LevelDescription(2000, Arrays.asList("Les assaillants perdent", "leur bouclier"))), "No Shield", Material.SHIELD),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.NO_SHIELD, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Les assaillants perdent", "leur bouclier")))), "No Shield", Material.SHIELD),</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -965,7 +1041,7 @@
       </c>
       <c r="D6" t="str" cm="1">
         <f t="array" ref="D6">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A6,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_STRENGH, Arrays.asList(new LevelDescription(500, Arrays.asList("Effet Force 1")), new LevelDescription(2000, Arrays.asList("Effet Force 1", "-&gt; Effet Force 2")), new LevelDescription(0, Arrays.asList("Effet Force 2"))), "Effet Force", Material.POTION),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_STRENGH, Arrays.asList(new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Effet Force 1"))), new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Effet Force 1", "-&gt; Effet Force 2"))), new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Effet Force 2")))), "Effet Force", Material.POTION),</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -980,7 +1056,7 @@
       </c>
       <c r="D7" t="str" cm="1">
         <f t="array" ref="D7">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A7,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_RESISTANCE, Arrays.asList(new LevelDescription(500, Arrays.asList("Effet Résistance 1")), new LevelDescription(2000, Arrays.asList("Effet Résistance 1", "-&gt;Effet Résistance 2")), new LevelDescription(0, Arrays.asList("Effet Résistance 2"))), "Effet Resistance", Material.POTION),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_RESISTANCE, Arrays.asList(new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Effet Résistance 1"))), new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Effet Résistance 1", "-&gt;Effet Résistance 2"))), new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Effet Résistance 2")))), "Effet Resistance", Material.POTION),</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -995,7 +1071,7 @@
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" ref="D8">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A8,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_SPEED, Arrays.asList(new LevelDescription(500, Arrays.asList("Effet Speed 1")), new LevelDescription(1000, Arrays.asList("Effet Speed 1", "-&gt;Effet Speed 2")), new LevelDescription(0, Arrays.asList("Effet Speed 2"))), "Effet Vitesse", Material.POTION),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_SPEED, Arrays.asList(new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Effet Speed 1"))), new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Effet Speed 1", "-&gt;Effet Speed 2"))), new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Effet Speed 2")))), "Effet Vitesse", Material.POTION),</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1010,7 +1086,7 @@
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" ref="D9">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A9,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_JUMP, Arrays.asList(new LevelDescription(500, Arrays.asList("Effet Jump 1")), new LevelDescription(1000, Arrays.asList("Effet Jump 1", "-&gt;Effet Jump 2")), new LevelDescription(0, Arrays.asList("Effet Jump 2"))), "Effet Saut", Material.POTION),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_JUMP, Arrays.asList(new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Effet Jump 1"))), new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Effet Jump 1", "-&gt;Effet Jump 2"))), new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Effet Jump 2")))), "Effet Saut", Material.POTION),</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1025,7 +1101,7 @@
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" ref="D10">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A10,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_FIRE_RESISTANCE, Arrays.asList(new LevelDescription(2000, Arrays.asList("Effet Résistance au Feu"))), "Effet Resistance au Feu", Material.BLAZE_POWDER),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_FIRE_RESISTANCE, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Effet Résistance au Feu")))), "Effet Resistance au Feu", Material.BLAZE_POWDER),</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1040,7 +1116,7 @@
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" ref="D11">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A11,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_WATER_BREATHING, Arrays.asList(new LevelDescription(500, Arrays.asList("Effet Respiration"))), "Effet Respiration", Material.CONDUIT),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_WATER_BREATHING, Arrays.asList(new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Effet Respiration")))), "Effet Respiration", Material.CONDUIT),</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1055,7 +1131,7 @@
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" ref="D12">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A12,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.MOB_FRIEND, Arrays.asList(new LevelDescription(500, Arrays.asList("Les mobs n'attaquent pas", "le capitaine"))), "Ami des Mobs", Material.CREEPER_HEAD),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.MOB_FRIEND, Arrays.asList(new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Les mobs n'attaquent pas", "le capitaine")))), "Ami des Mobs", Material.CREEPER_HEAD),</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1068,9 +1144,9 @@
       <c r="C13" t="s">
         <v>61</v>
       </c>
-      <c r="D13" t="str" cm="1">
+      <c r="D13" t="e" cm="1" vm="1">
         <f t="array" ref="D13">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A13,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.ENNEMY_DETECTION, Arrays.asList(new LevelDescription(2000, Arrays.asList("Les assaillants à moins", "de 30 blocs sont en", "surbrillance"))), "Detection des assaillants", Material.TARGET),</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1085,7 +1161,7 @@
       </c>
       <c r="D14" t="str" cm="1">
         <f t="array" ref="D14">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A14,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.NO_FALL_DAMAGE, Arrays.asList(new LevelDescription(2000, Arrays.asList("Pas de dégât de chute"))), "Pas de chute", Material.FEATHER),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.NO_FALL_DAMAGE, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Pas de dégât de chute")))), "Pas de chute", Material.FEATHER),</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1100,7 +1176,7 @@
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" ref="D15">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A15,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SCREAM, Arrays.asList(new LevelDescription(1000, Arrays.asList("Envoi les ennemis proches", "dans les airs"))), "Sort : Cri d'Effroi", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SCREAM, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Envoi les ennemis proches", "dans les airs")))), "Sort : Cri d'Effroi", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1115,7 +1191,7 @@
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" ref="D16">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A16,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SUMMON, Arrays.asList(new LevelDescription(1000, Arrays.asList("Invoque des mobs près", "des assaillants"))), "Sort : Invocation", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SUMMON, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Invoque des mobs près", "des assaillants")))), "Sort : Invocation", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1130,7 +1206,7 @@
       </c>
       <c r="D17" t="str" cm="1">
         <f t="array" ref="D17">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A17,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_JUMP, Arrays.asList(new LevelDescription(1000, Arrays.asList("Fait un grand saut"))), "Sort : Saut", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_JUMP, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Fait un grand saut")))), "Sort : Saut", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1145,7 +1221,7 @@
       </c>
       <c r="D18" t="str" cm="1">
         <f t="array" ref="D18">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A18,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_EXPLOSIVE_PUN, Arrays.asList(new LevelDescription(2000, Arrays.asList("Le prochain bloc posé", "par un assaillant explose"))), "Sort : Farce Explosive", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_EXPLOSIVE_PUN, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Le prochain bloc posé", "par un assaillant explose")))), "Sort : Farce Explosive", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,7 +1236,7 @@
       </c>
       <c r="D19" t="str" cm="1">
         <f t="array" ref="D19">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A19,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_JAIL, Arrays.asList(new LevelDescription(2000, Arrays.asList("Enferme tous les  assaillants", "dans une prison d'obsidienne"))), "Sort : Prison", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_JAIL, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Enferme tous les  assaillants", "dans une prison d'obsidienne")))), "Sort : Prison", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,7 +1251,7 @@
       </c>
       <c r="D20" t="str" cm="1">
         <f t="array" ref="D20">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A20,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_ADIOS, Arrays.asList(new LevelDescription(2000, Arrays.asList("Fait disparaitre tous les", "blocs sous les pieds du", "capitaine jusqu'à la couche 0"))), "Sort : Adios!", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_ADIOS, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Fait disparaitre tous les", "blocs sous les pieds du", "capitaine jusqu'à la couche 0")))), "Sort : Adios!", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1190,7 +1266,7 @@
       </c>
       <c r="D21" t="str" cm="1">
         <f t="array" ref="D21">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A21,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SHUFFLE, Arrays.asList(new LevelDescription(1000, Arrays.asList("Intervertit la position", "des assaillants"))), "Sort : Shuffle", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SHUFFLE, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Intervertit la position", "des assaillants")))), "Sort : Shuffle", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1205,7 +1281,7 @@
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" ref="D22">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A22,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_REVIVE, Arrays.asList(new LevelDescription(2000, Arrays.asList("A 0 cœurs récupère", "3 cœurs + 2 d'abso", "un assaillant allié perd", "tout son équipement"))), "Sauvetage", Material.TOTEM_OF_UNDYING),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_REVIVE, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("A 0 cœurs récupère", "3 cœurs + 2 d'abso", "un assaillant allié perd", "tout son équipement")))), "Sauvetage", Material.TOTEM_OF_UNDYING),</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1220,7 +1296,7 @@
       </c>
       <c r="D23" t="str" cm="1">
         <f t="array" ref="D23">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A23,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_BALANCE, Arrays.asList(new LevelDescription(4000, Arrays.asList("A 5 cœurs les assaillants", "subissent un poison jusqu'à", "5 cœurs max"))), "Equilibre", Material.DAMAGED_ANVIL),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_BALANCE, Arrays.asList(new LevelDescription(4000, new ArrayList&lt;&gt;(Arrays.asList("A 5 cœurs les assaillants", "subissent un poison jusqu'à", "5 cœurs max")))), "Equilibre", Material.DAMAGED_ANVIL),</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1235,7 +1311,7 @@
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" ref="D24">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A24,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_JUMP_SCARE, Arrays.asList(new LevelDescription(2000, Arrays.asList("A 2 cœurs teleporte", "le capitaine au point le", "plus haut de sa position"))), "Trouille", Material.JACK_O_LANTERN),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_JUMP_SCARE, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("A 2 cœurs teleporte", "le capitaine au point le", "plus haut de sa position")))), "Trouille", Material.JACK_O_LANTERN),</v>
       </c>
     </row>
   </sheetData>
@@ -1252,7 +1328,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,8 +1370,8 @@
         <v>67</v>
       </c>
       <c r="E2" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(10, Arrays.asList("Equipement Cuir et Pierre"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(10, new ArrayList&lt;&gt;(Arrays.asList("Equipement Cuir et Pierre")))</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1313,8 +1389,8 @@
         <v>68</v>
       </c>
       <c r="E3" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(20, Arrays.asList("Equipement Cuir et Pierre", "-&gt; Equipement Or"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(20, new ArrayList&lt;&gt;(Arrays.asList("Equipement Cuir et Pierre", "-&gt; Equipement Or")))</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1332,8 +1408,8 @@
         <v>69</v>
       </c>
       <c r="E4" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(50, Arrays.asList("Equipement Or", "-&gt; Equipement Fer"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(50, new ArrayList&lt;&gt;(Arrays.asList("Equipement Or", "-&gt; Equipement Fer")))</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1351,8 +1427,8 @@
         <v>70</v>
       </c>
       <c r="E5" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(100, Arrays.asList("Equipement Fer", "-&gt; Equipement Diamant"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(100, new ArrayList&lt;&gt;(Arrays.asList("Equipement Fer", "-&gt; Equipement Diamant")))</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1370,8 +1446,8 @@
         <v>71</v>
       </c>
       <c r="E6" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(200, Arrays.asList("Equipement Diamant", "-&gt; Equipement Netherite"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(200, new ArrayList&lt;&gt;(Arrays.asList("Equipement Diamant", "-&gt; Equipement Netherite")))</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1389,8 +1465,8 @@
         <v>73</v>
       </c>
       <c r="E7" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(200, Arrays.asList("Equipement Netherite", "-&gt; Protection 1"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(200, new ArrayList&lt;&gt;(Arrays.asList("Equipement Netherite", "-&gt; Protection 1")))</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1408,8 +1484,8 @@
         <v>74</v>
       </c>
       <c r="E8" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(300, Arrays.asList("Protection 1", "-&gt; Protection 2"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(300, new ArrayList&lt;&gt;(Arrays.asList("Protection 1", "-&gt; Protection 2")))</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1427,8 +1503,8 @@
         <v>75</v>
       </c>
       <c r="E9" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(400, Arrays.asList("Protection 2", "-&gt; Protection 3"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(400, new ArrayList&lt;&gt;(Arrays.asList("Protection 2", "-&gt; Protection 3")))</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,8 +1522,8 @@
         <v>76</v>
       </c>
       <c r="E10" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(500, Arrays.asList("Protection 3", "-&gt;Protection 4"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Protection 3", "-&gt;Protection 4")))</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1465,8 +1541,8 @@
         <v>77</v>
       </c>
       <c r="E11" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(200, Arrays.asList("Protection 4", "-&gt; Full Enchant"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(200, new ArrayList&lt;&gt;(Arrays.asList("Protection 4", "-&gt; Full Enchant")))</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,8 +1559,8 @@
         <v>78</v>
       </c>
       <c r="E12" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(0, Arrays.asList("Full Enchant"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Full Enchant")))</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1501,8 +1577,8 @@
         <v>79</v>
       </c>
       <c r="E13" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(50, Arrays.asList("Arc + 2 stacks de Fleches"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(50, new ArrayList&lt;&gt;(Arrays.asList("Arc + 2 stacks de Fleches")))</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1520,8 +1596,8 @@
         <v>80</v>
       </c>
       <c r="E14" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(100, Arrays.asList("Arc + 2 stacks de Fleches", "-&gt;Power 1"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(100, new ArrayList&lt;&gt;(Arrays.asList("Arc + 2 stacks de Fleches", "-&gt;Power 1")))</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,8 +1615,8 @@
         <v>81</v>
       </c>
       <c r="E15" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(300, Arrays.asList("Power 1", "-&gt; Power 3 + 1 stack de Flèches"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(300, new ArrayList&lt;&gt;(Arrays.asList("Power 1", "-&gt; Power 3 + 1 stack de Flèches")))</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1558,8 +1634,8 @@
         <v>83</v>
       </c>
       <c r="E16" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(200, Arrays.asList("Power 3 + 1 stack de Flèches", "-&gt; Power 4"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(200, new ArrayList&lt;&gt;(Arrays.asList("Power 3 + 1 stack de Flèches", "-&gt; Power 4")))</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1577,8 +1653,8 @@
         <v>82</v>
       </c>
       <c r="E17" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(500, Arrays.asList("Power 4", "-&gt; Full Enchant"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Power 4", "-&gt; Full Enchant")))</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1595,8 +1671,8 @@
         <v>78</v>
       </c>
       <c r="E18" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(0, Arrays.asList("Full Enchant"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Full Enchant")))</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1613,8 +1689,8 @@
         <v>84</v>
       </c>
       <c r="E19" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(500, Arrays.asList("Recoit les items de", "son Ender Chest"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Recoit les items de", "son Ender Chest")))</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1631,8 +1707,8 @@
         <v>85</v>
       </c>
       <c r="E20" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("Les assaillants perdent", "leur bouclier"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Les assaillants perdent", "leur bouclier")))</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1649,8 +1725,8 @@
         <v>86</v>
       </c>
       <c r="E21" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(500, Arrays.asList("Effet Force 1"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Effet Force 1")))</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1667,8 +1743,8 @@
         <v>87</v>
       </c>
       <c r="E22" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("Effet Force 1", "-&gt; Effet Force 2"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Effet Force 1", "-&gt; Effet Force 2")))</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1685,8 +1761,8 @@
         <v>88</v>
       </c>
       <c r="E23" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(0, Arrays.asList("Effet Force 2"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Effet Force 2")))</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1703,8 +1779,8 @@
         <v>89</v>
       </c>
       <c r="E24" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(500, Arrays.asList("Effet Résistance 1"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Effet Résistance 1")))</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1721,8 +1797,8 @@
         <v>90</v>
       </c>
       <c r="E25" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("Effet Résistance 1", "-&gt;Effet Résistance 2"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Effet Résistance 1", "-&gt;Effet Résistance 2")))</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1739,8 +1815,8 @@
         <v>91</v>
       </c>
       <c r="E26" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(0, Arrays.asList("Effet Résistance 2"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Effet Résistance 2")))</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1757,8 +1833,8 @@
         <v>92</v>
       </c>
       <c r="E27" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(500, Arrays.asList("Effet Speed 1"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Effet Speed 1")))</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1775,8 +1851,8 @@
         <v>93</v>
       </c>
       <c r="E28" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(1000, Arrays.asList("Effet Speed 1", "-&gt;Effet Speed 2"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Effet Speed 1", "-&gt;Effet Speed 2")))</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1793,8 +1869,8 @@
         <v>94</v>
       </c>
       <c r="E29" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(0, Arrays.asList("Effet Speed 2"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Effet Speed 2")))</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1811,8 +1887,8 @@
         <v>95</v>
       </c>
       <c r="E30" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(500, Arrays.asList("Effet Jump 1"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Effet Jump 1")))</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1829,8 +1905,8 @@
         <v>96</v>
       </c>
       <c r="E31" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(1000, Arrays.asList("Effet Jump 1", "-&gt;Effet Jump 2"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Effet Jump 1", "-&gt;Effet Jump 2")))</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1847,8 +1923,8 @@
         <v>97</v>
       </c>
       <c r="E32" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(0, Arrays.asList("Effet Jump 2"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(0, new ArrayList&lt;&gt;(Arrays.asList("Effet Jump 2")))</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1865,8 +1941,8 @@
         <v>98</v>
       </c>
       <c r="E33" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("Effet Résistance au Feu"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Effet Résistance au Feu")))</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1883,8 +1959,8 @@
         <v>40</v>
       </c>
       <c r="E34" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(500, Arrays.asList("Effet Respiration"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Effet Respiration")))</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1901,13 +1977,13 @@
         <v>99</v>
       </c>
       <c r="E35" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(500, Arrays.asList("Les mobs n'attaquent pas", "le capitaine"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Les mobs n'attaquent pas", "le capitaine")))</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1919,8 +1995,8 @@
         <v>100</v>
       </c>
       <c r="E36" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("Les assaillants à moins", "de 30 blocs sont en", "surbrillance"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Les assaillants à moins", "de 30 blocs sont en", "surbrillance")))</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1937,8 +2013,8 @@
         <v>101</v>
       </c>
       <c r="E37" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("Pas de dégât de chute"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Pas de dégât de chute")))</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1955,8 +2031,8 @@
         <v>102</v>
       </c>
       <c r="E38" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(1000, Arrays.asList("Envoi les ennemis proches", "dans les airs"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Envoi les ennemis proches", "dans les airs")))</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1973,8 +2049,8 @@
         <v>103</v>
       </c>
       <c r="E39" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(1000, Arrays.asList("Invoque des mobs près", "des assaillants"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Invoque des mobs près", "des assaillants")))</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1991,8 +2067,8 @@
         <v>104</v>
       </c>
       <c r="E40" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(1000, Arrays.asList("Fait un grand saut"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Fait un grand saut")))</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2009,8 +2085,8 @@
         <v>105</v>
       </c>
       <c r="E41" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("Le prochain bloc posé", "par un assaillant explose"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Le prochain bloc posé", "par un assaillant explose")))</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2027,8 +2103,8 @@
         <v>111</v>
       </c>
       <c r="E42" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("Enferme tous les  assaillants", "dans une prison d'obsidienne"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Enferme tous les  assaillants", "dans une prison d'obsidienne")))</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2045,8 +2121,8 @@
         <v>106</v>
       </c>
       <c r="E43" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("Fait disparaitre tous les", "blocs sous les pieds du", "capitaine jusqu'à la couche 0"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Fait disparaitre tous les", "blocs sous les pieds du", "capitaine jusqu'à la couche 0")))</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2063,8 +2139,8 @@
         <v>107</v>
       </c>
       <c r="E44" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(1000, Arrays.asList("Intervertit la position", "des assaillants"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Intervertit la position", "des assaillants")))</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2081,8 +2157,8 @@
         <v>108</v>
       </c>
       <c r="E45" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("A 0 cœurs récupère", "3 cœurs + 2 d'abso", "un assaillant allié perd", "tout son équipement"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("A 0 cœurs récupère", "3 cœurs + 2 d'abso", "un assaillant allié perd", "tout son équipement")))</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2099,8 +2175,8 @@
         <v>109</v>
       </c>
       <c r="E46" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(4000, Arrays.asList("A 5 cœurs les assaillants", "subissent un poison jusqu'à", "5 cœurs max"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(4000, new ArrayList&lt;&gt;(Arrays.asList("A 5 cœurs les assaillants", "subissent un poison jusqu'à", "5 cœurs max")))</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2117,14 +2193,15 @@
         <v>110</v>
       </c>
       <c r="E47" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),"))")</f>
-        <v>new LevelDescription(2000, Arrays.asList("A 2 cœurs teleporte", "le capitaine au point le", "plus haut de sa position"))</v>
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("A 2 cœurs teleporte", "le capitaine au point le", "plus haut de sa position")))</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrections + add saturation power
</commit_message>
<xml_diff>
--- a/powerandprice.xlsx
+++ b/powerandprice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projets Prog\GitHub\FlamboyantSurvivalRumble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D12A3B-3DD8-4B43-806E-378716FDFA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DC229A-2395-433C-943D-F1EFF80F2E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE0511E6-2CB4-423D-9419-747EC9372C3E}"/>
   </bookViews>
@@ -38,9 +38,8 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
+  <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -51,30 +50,16 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="116">
   <si>
     <t>EQUIPMENT</t>
   </si>
@@ -109,9 +94,6 @@
     <t>MOB_FRIEND</t>
   </si>
   <si>
-    <t>ENNEMY_DETECTION</t>
-  </si>
-  <si>
     <t>NO_FALL_DAMAGE</t>
   </si>
   <si>
@@ -412,7 +394,19 @@
     <t>Enferme tous les  assaillants|dans une prison d'obsidienne</t>
   </si>
   <si>
-    <t>ENNEMIES_DETECTION</t>
+    <t>EFFECT_SATURATION</t>
+  </si>
+  <si>
+    <t>Saturation</t>
+  </si>
+  <si>
+    <t>COOKED_BEEF</t>
+  </si>
+  <si>
+    <t>Effet Saturation</t>
+  </si>
+  <si>
+    <t>ENEMIES_DETECTION</t>
   </si>
 </sst>
 </file>
@@ -465,10 +459,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,67 +532,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>13</v>
-    <v>3</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_error">
-    <k n="errorType" t="i"/>
-    <k n="subType" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB36BB41-6156-43AD-97FF-A9DAF9EB0FFB}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0">
-  <autoFilter ref="A1:D24" xr:uid="{DB36BB41-6156-43AD-97FF-A9DAF9EB0FFB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB36BB41-6156-43AD-97FF-A9DAF9EB0FFB}" name="Tableau1" displayName="Tableau1" ref="A1:D25" totalsRowShown="0">
+  <autoFilter ref="A1:D25" xr:uid="{DB36BB41-6156-43AD-97FF-A9DAF9EB0FFB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{6C46DAC8-560F-4C0E-A953-82498D3166C8}" name="Effect enum"/>
     <tableColumn id="4" xr3:uid="{B62B264B-1F8F-4BBC-8B19-926F7AB01D18}" name="Name"/>
@@ -610,8 +548,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2796FCD-5C41-4103-9DBE-EF9DFB53ACDC}" name="Tableau3" displayName="Tableau3" ref="A1:E47" totalsRowShown="0" tableBorderDxfId="2">
-  <autoFilter ref="A1:E47" xr:uid="{D2796FCD-5C41-4103-9DBE-EF9DFB53ACDC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2796FCD-5C41-4103-9DBE-EF9DFB53ACDC}" name="Tableau3" displayName="Tableau3" ref="A1:E48" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="A1:E48" xr:uid="{D2796FCD-5C41-4103-9DBE-EF9DFB53ACDC}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8F341F71-2B53-409D-83BA-B4D0D14E06C7}" name="Effect enum" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{34497726-02A4-4E64-A7CC-3DEB45AF79C3}" name="Level"/>
@@ -942,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF46C1E-7778-41FA-B71C-06D6E1FA3772}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,16 +895,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -974,10 +912,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" t="str" cm="1">
         <f t="array" ref="D2">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A2,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
@@ -989,7 +927,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1004,10 +942,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" t="str" cm="1">
         <f t="array" ref="D4">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A4,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
@@ -1019,10 +957,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" t="str" cm="1">
         <f t="array" ref="D5">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A5,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
@@ -1034,10 +972,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" t="str" cm="1">
         <f t="array" ref="D6">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A6,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
@@ -1049,10 +987,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" t="str" cm="1">
         <f t="array" ref="D7">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A7,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
@@ -1064,10 +1002,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" ref="D8">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A8,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
@@ -1079,10 +1017,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" ref="D9">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A9,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
@@ -1094,10 +1032,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" ref="D10">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A10,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
@@ -1109,10 +1047,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" ref="D11">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A11,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
@@ -1121,196 +1059,211 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" t="str" cm="1">
+        <v>113</v>
+      </c>
+      <c r="D12" s="4" t="str" cm="1">
         <f t="array" ref="D12">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A12,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.MOB_FRIEND, Arrays.asList(new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Les mobs n'attaquent pas", "le capitaine")))), "Ami des Mobs", Material.CREEPER_HEAD),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.EFFECT_SATURATION, Arrays.asList(new LevelDescription(100, new ArrayList&lt;&gt;(Arrays.asList("Effet Saturation")))), "Saturation", Material.COOKED_BEEF),</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" t="e" cm="1" vm="1">
+        <v>59</v>
+      </c>
+      <c r="D13" t="str" cm="1">
         <f t="array" ref="D13">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A13,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>#VALUE!</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.MOB_FRIEND, Arrays.asList(new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Les mobs n'attaquent pas", "le capitaine")))), "Ami des Mobs", Material.CREEPER_HEAD),</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D14" t="str" cm="1">
         <f t="array" ref="D14">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A14,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.NO_FALL_DAMAGE, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Pas de dégât de chute")))), "Pas de chute", Material.FEATHER),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.ENEMIES_DETECTION, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Les assaillants à moins", "de 30 blocs sont en", "surbrillance")))), "Detection des assaillants", Material.TARGET),</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" ref="D15">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A15,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SCREAM, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Envoi les ennemis proches", "dans les airs")))), "Sort : Cri d'Effroi", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.NO_FALL_DAMAGE, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Pas de dégât de chute")))), "Pas de chute", Material.FEATHER),</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" ref="D16">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A16,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SUMMON, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Invoque des mobs près", "des assaillants")))), "Sort : Invocation", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SCREAM, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Envoi les ennemis proches", "dans les airs")))), "Sort : Cri d'Effroi", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" t="str" cm="1">
         <f t="array" ref="D17">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A17,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_JUMP, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Fait un grand saut")))), "Sort : Saut", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SUMMON, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Invoque des mobs près", "des assaillants")))), "Sort : Invocation", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" t="str" cm="1">
         <f t="array" ref="D18">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A18,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_EXPLOSIVE_PUN, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Le prochain bloc posé", "par un assaillant explose")))), "Sort : Farce Explosive", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_JUMP, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Fait un grand saut")))), "Sort : Saut", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" t="str" cm="1">
         <f t="array" ref="D19">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A19,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_JAIL, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Enferme tous les  assaillants", "dans une prison d'obsidienne")))), "Sort : Prison", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_EXPLOSIVE_PUN, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Le prochain bloc posé", "par un assaillant explose")))), "Sort : Farce Explosive", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" t="str" cm="1">
         <f t="array" ref="D20">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A20,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_ADIOS, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Fait disparaitre tous les", "blocs sous les pieds du", "capitaine jusqu'à la couche 0")))), "Sort : Adios!", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_JAIL, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Enferme tous les  assaillants", "dans une prison d'obsidienne")))), "Sort : Prison", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" t="str" cm="1">
         <f t="array" ref="D21">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A21,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SHUFFLE, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Intervertit la position", "des assaillants")))), "Sort : Shuffle", Material.WRITABLE_BOOK),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_ADIOS, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Fait disparaitre tous les", "blocs sous les pieds du", "capitaine jusqu'à la couche 0")))), "Sort : Adios!", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" ref="D22">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A22,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_REVIVE, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("A 0 cœurs récupère", "3 cœurs + 2 d'abso", "un assaillant allié perd", "tout son équipement")))), "Sauvetage", Material.TOTEM_OF_UNDYING),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.SPELL_SHUFFLE, Arrays.asList(new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Intervertit la position", "des assaillants")))), "Sort : Shuffle", Material.WRITABLE_BOOK),</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D23" t="str" cm="1">
         <f t="array" ref="D23">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A23,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
-        <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_BALANCE, Arrays.asList(new LevelDescription(4000, new ArrayList&lt;&gt;(Arrays.asList("A 5 cœurs les assaillants", "subissent un poison jusqu'à", "5 cœurs max")))), "Equilibre", Material.DAMAGED_ANVIL),</v>
+        <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_REVIVE, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("A 0 cœurs récupère", "3 cœurs + 2 d'abso", "un assaillant allié perd", "tout son équipement")))), "Sauvetage", Material.TOTEM_OF_UNDYING),</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" ref="D24">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A24,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
+        <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_BALANCE, Arrays.asList(new LevelDescription(4000, new ArrayList&lt;&gt;(Arrays.asList("A 5 cœurs les assaillants", "subissent un poison jusqu'à", "5 cœurs max")))), "Equilibre", Material.DAMAGED_ANVIL),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="str" cm="1">
+        <f t="array" ref="D25">_xlfn.CONCAT("new ChampionPowerShopItem(ChampionPowerType.",A25,", Arrays.asList(",_xlfn.TEXTJOIN(", ", TRUE, _xlfn._xlws.FILTER(Tableau3[Quoted], Tableau3[Effect enum]=Tableau1[[#This Row],[Effect enum]])),"), ",CHAR(34),Tableau1[[#This Row],[Name]],CHAR(34),", Material.",Tableau1[[#This Row],[Material]],"),")</f>
         <v>new ChampionPowerShopItem(ChampionPowerType.COME_BACK_JUMP_SCARE, Arrays.asList(new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("A 2 cœurs teleporte", "le capitaine au point le", "plus haut de sa position")))), "Trouille", Material.JACK_O_LANTERN),</v>
       </c>
     </row>
@@ -1325,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D50422-CDA8-489F-BE44-C27697BFE280}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,19 +1294,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1367,7 +1320,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1386,7 +1339,7 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1405,7 +1358,7 @@
         <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1424,7 +1377,7 @@
         <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1443,7 +1396,7 @@
         <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1462,7 +1415,7 @@
         <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1481,7 +1434,7 @@
         <v>300</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1500,7 +1453,7 @@
         <v>400</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1519,7 +1472,7 @@
         <v>500</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E10" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1538,7 +1491,7 @@
         <v>200</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E11" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1550,13 +1503,13 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1574,7 +1527,7 @@
         <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1593,7 +1546,7 @@
         <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1612,7 +1565,7 @@
         <v>300</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1631,7 +1584,7 @@
         <v>200</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1650,7 +1603,7 @@
         <v>500</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1662,13 +1615,13 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1686,7 +1639,7 @@
         <v>500</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1704,7 +1657,7 @@
         <v>2000</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E20" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1722,7 +1675,7 @@
         <v>500</v>
       </c>
       <c r="D21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1740,7 +1693,7 @@
         <v>2000</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1752,13 +1705,13 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1776,7 +1729,7 @@
         <v>500</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E24" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1794,7 +1747,7 @@
         <v>2000</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1806,13 +1759,13 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1830,7 +1783,7 @@
         <v>500</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E27" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1848,7 +1801,7 @@
         <v>1000</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E28" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1860,13 +1813,13 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E29" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1884,7 +1837,7 @@
         <v>500</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E30" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1902,7 +1855,7 @@
         <v>1000</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E31" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1914,13 +1867,13 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E32" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1938,7 +1891,7 @@
         <v>2000</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E33" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1956,7 +1909,7 @@
         <v>500</v>
       </c>
       <c r="D34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
@@ -1964,44 +1917,44 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>100</v>
+      </c>
+      <c r="D35" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="4" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(100, new ArrayList&lt;&gt;(Arrays.asList("Effet Saturation")))</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
         <v>500</v>
       </c>
-      <c r="D35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E35" t="str">
+      <c r="D36" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
         <v>new LevelDescription(500, new ArrayList&lt;&gt;(Arrays.asList("Les mobs n'attaquent pas", "le capitaine")))</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>2000</v>
-      </c>
-      <c r="D36" t="s">
-        <v>100</v>
-      </c>
-      <c r="E36" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
-        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Les assaillants à moins", "de 30 blocs sont en", "surbrillance")))</v>
-      </c>
-    </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>12</v>
+      <c r="A37" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -2010,34 +1963,34 @@
         <v>2000</v>
       </c>
       <c r="D37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E37" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Les assaillants à moins", "de 30 blocs sont en", "surbrillance")))</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>2000</v>
+      </c>
+      <c r="D38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
         <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Pas de dégât de chute")))</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>1000</v>
-      </c>
-      <c r="D38" t="s">
-        <v>102</v>
-      </c>
-      <c r="E38" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
-        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Envoi les ennemis proches", "dans les airs")))</v>
-      </c>
-    </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>14</v>
+      <c r="A39" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2046,16 +1999,16 @@
         <v>1000</v>
       </c>
       <c r="D39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E39" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
-        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Invoque des mobs près", "des assaillants")))</v>
+        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Envoi les ennemis proches", "dans les airs")))</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>15</v>
+      <c r="A40" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2064,34 +2017,34 @@
         <v>1000</v>
       </c>
       <c r="D40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E40" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Invoque des mobs près", "des assaillants")))</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1000</v>
+      </c>
+      <c r="D41" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
         <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Fait un grand saut")))</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>2000</v>
-      </c>
-      <c r="D41" t="s">
-        <v>105</v>
-      </c>
-      <c r="E41" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
-        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Le prochain bloc posé", "par un assaillant explose")))</v>
-      </c>
-    </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>17</v>
+      <c r="A42" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2100,16 +2053,16 @@
         <v>2000</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E42" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
-        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Enferme tous les  assaillants", "dans une prison d'obsidienne")))</v>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Le prochain bloc posé", "par un assaillant explose")))</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>18</v>
+      <c r="A43" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2118,81 +2071,99 @@
         <v>2000</v>
       </c>
       <c r="D43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Enferme tous les  assaillants", "dans une prison d'obsidienne")))</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>2000</v>
+      </c>
+      <c r="D44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Fait disparaitre tous les", "blocs sous les pieds du", "capitaine jusqu'à la couche 0")))</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1000</v>
+      </c>
+      <c r="D45" t="s">
         <v>106</v>
       </c>
-      <c r="E43" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
-        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("Fait disparaitre tous les", "blocs sous les pieds du", "capitaine jusqu'à la couche 0")))</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="E45" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Intervertit la position", "des assaillants")))</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>1000</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>2000</v>
+      </c>
+      <c r="D46" t="s">
         <v>107</v>
       </c>
-      <c r="E44" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
-        <v>new LevelDescription(1000, new ArrayList&lt;&gt;(Arrays.asList("Intervertit la position", "des assaillants")))</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="E46" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("A 0 cœurs récupère", "3 cœurs + 2 d'abso", "un assaillant allié perd", "tout son équipement")))</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>4000</v>
+      </c>
+      <c r="D47" t="s">
+        <v>108</v>
+      </c>
+      <c r="E47" t="str">
+        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
+        <v>new LevelDescription(4000, new ArrayList&lt;&gt;(Arrays.asList("A 5 cœurs les assaillants", "subissent un poison jusqu'à", "5 cœurs max")))</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
         <v>2000</v>
       </c>
-      <c r="D45" t="s">
-        <v>108</v>
-      </c>
-      <c r="E45" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
-        <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("A 0 cœurs récupère", "3 cœurs + 2 d'abso", "un assaillant allié perd", "tout son équipement")))</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>4000</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>109</v>
       </c>
-      <c r="E46" t="str">
-        <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
-        <v>new LevelDescription(4000, new ArrayList&lt;&gt;(Arrays.asList("A 5 cœurs les assaillants", "subissent un poison jusqu'à", "5 cœurs max")))</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>2000</v>
-      </c>
-      <c r="D47" t="s">
-        <v>110</v>
-      </c>
-      <c r="E47" t="str">
+      <c r="E48" t="str">
         <f>_xlfn.CONCAT("new LevelDescription(",Tableau3[[#This Row],[Price]],", new ArrayList&lt;&gt;(Arrays.asList(",CHAR(34),SUBSTITUTE(Tableau3[[#This Row],[Description]], "|", _xlfn.CONCAT(CHAR(34),", ", CHAR(34))),CHAR(34),")))")</f>
         <v>new LevelDescription(2000, new ArrayList&lt;&gt;(Arrays.asList("A 2 cœurs teleporte", "le capitaine au point le", "plus haut de sa position")))</v>
       </c>

</xml_diff>